<commit_message>
Implemented single level JSR and RTS
</commit_message>
<xml_diff>
--- a/Docs/CPU_Opcodes.xlsx
+++ b/Docs/CPU_Opcodes.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="104">
   <si>
     <t xml:space="preserve">INSTRUCTION</t>
   </si>
@@ -350,6 +350,7 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -367,12 +368,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -416,7 +423,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -453,6 +460,34 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -473,10 +508,10 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="5.04"/>
@@ -1268,7 +1303,7 @@
       <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.16"/>
@@ -1448,10 +1483,10 @@
   <dimension ref="A1:R1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="4.83"/>
@@ -1685,114 +1720,215 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
+    <row r="7" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" s="10"/>
+      <c r="H7" s="10"/>
+      <c r="I7" s="10"/>
+      <c r="J7" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="K7" s="10"/>
+      <c r="L7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="10"/>
+      <c r="Q7" s="10"/>
+      <c r="R7" s="11" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+      <c r="N8" s="14"/>
+      <c r="O8" s="14"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="14"/>
+      <c r="R8" s="15"/>
+    </row>
+    <row r="9" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="13" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="13" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="13" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+      <c r="N9" s="14"/>
+      <c r="O9" s="14"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="14"/>
+      <c r="R9" s="15"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="B10" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="5" t="s">
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+      <c r="J10" s="3"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+      <c r="M10" s="3"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+      <c r="R10" s="5" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="B8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D8" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F8" s="3" t="s">
+      <c r="B11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E11" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="5" t="s">
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+      <c r="R11" s="5" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B9" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D9" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="B12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D12" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="G9" s="3"/>
-      <c r="H9" s="3"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="5" t="s">
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+      <c r="J12" s="3"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+      <c r="M12" s="3"/>
+      <c r="N12" s="3"/>
+      <c r="O12" s="3"/>
+      <c r="P12" s="3"/>
+      <c r="Q12" s="3"/>
+      <c r="R12" s="5" t="s">
         <v>46</v>
       </c>
     </row>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="20">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
@@ -1806,9 +1942,13 @@
     <mergeCell ref="J5:Q5"/>
     <mergeCell ref="F6:I6"/>
     <mergeCell ref="J6:Q6"/>
-    <mergeCell ref="F7:Q7"/>
+    <mergeCell ref="F7:I7"/>
+    <mergeCell ref="J7:Q7"/>
     <mergeCell ref="F8:Q8"/>
     <mergeCell ref="F9:Q9"/>
+    <mergeCell ref="F10:Q10"/>
+    <mergeCell ref="F11:Q11"/>
+    <mergeCell ref="F12:Q12"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Fixed Assembler external dependencies
</commit_message>
<xml_diff>
--- a/Docs/CPU_Opcodes.xlsx
+++ b/Docs/CPU_Opcodes.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="110">
   <si>
     <t xml:space="preserve">INSTRUCTION</t>
   </si>
@@ -335,6 +335,24 @@
   </si>
   <si>
     <t xml:space="preserve">I2C Control</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JUMP TO SUBROUTINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RETURN FROM SUBROUTINE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PSUEDO-OPS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0X8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HLT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HALT</t>
   </si>
 </sst>
 </file>
@@ -368,18 +386,12 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor rgb="FFFFFF00"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -423,7 +435,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -472,22 +484,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -508,10 +504,10 @@
   <dimension ref="A1:R19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="A16:R19 A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.36"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="2" style="1" width="5.04"/>
@@ -1049,7 +1045,7 @@
   <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="1" sqref="A16:R19 D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1300,10 +1296,10 @@
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H5" activeCellId="0" sqref="H5"/>
+      <selection pane="topLeft" activeCell="H5" activeCellId="1" sqref="A16:R19 H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.16"/>
@@ -1483,10 +1479,10 @@
   <dimension ref="A1:R1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="A16" activeCellId="0" sqref="A16:R19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="4.83"/>
@@ -1720,105 +1716,109 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="9" t="s">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B7" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="D7" s="9" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="B7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D7" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10" t="s">
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
-      <c r="M7" s="10"/>
-      <c r="N7" s="10"/>
-      <c r="O7" s="10"/>
-      <c r="P7" s="10"/>
-      <c r="Q7" s="10"/>
-      <c r="R7" s="11" t="s">
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+      <c r="M7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="R7" s="5" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="8" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="9" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D8" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="F8" s="14" t="s">
+      <c r="B8" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D8" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E8" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
-      <c r="I8" s="14"/>
-      <c r="J8" s="14"/>
-      <c r="K8" s="14"/>
-      <c r="L8" s="14"/>
-      <c r="M8" s="14"/>
-      <c r="N8" s="14"/>
-      <c r="O8" s="14"/>
-      <c r="P8" s="14"/>
-      <c r="Q8" s="14"/>
-      <c r="R8" s="15"/>
-    </row>
-    <row r="9" s="12" customFormat="true" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="13" t="s">
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="J8" s="10"/>
+      <c r="K8" s="10"/>
+      <c r="L8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="B9" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="C9" s="13" t="n">
-        <v>0</v>
-      </c>
-      <c r="D9" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" s="13" t="n">
-        <v>1</v>
-      </c>
-      <c r="F9" s="14" t="s">
+      <c r="B9" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="9" t="n">
+        <v>0</v>
+      </c>
+      <c r="D9" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="14"/>
-      <c r="M9" s="14"/>
-      <c r="N9" s="14"/>
-      <c r="O9" s="14"/>
-      <c r="P9" s="14"/>
-      <c r="Q9" s="14"/>
-      <c r="R9" s="15"/>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="J9" s="10"/>
+      <c r="K9" s="10"/>
+      <c r="L9" s="10"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="11" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
@@ -1836,20 +1836,20 @@
       <c r="E10" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
+      <c r="F10" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="J10" s="10"/>
+      <c r="K10" s="10"/>
+      <c r="L10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
       <c r="R10" s="5" t="s">
         <v>42</v>
       </c>
@@ -1870,20 +1870,20 @@
       <c r="E11" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="G11" s="3"/>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
+      <c r="F11" s="10" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10"/>
+      <c r="L11" s="10"/>
+      <c r="M11" s="10"/>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
       <c r="R11" s="5" t="s">
         <v>44</v>
       </c>
@@ -1922,13 +1922,170 @@
         <v>46</v>
       </c>
     </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="3"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="3"/>
+      <c r="P16" s="3"/>
+      <c r="Q16" s="3"/>
+      <c r="R16" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="2"/>
+      <c r="B17" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="L17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="M17" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="N17" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="O17" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="P17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q17" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="R17" s="2"/>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B18" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D18" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E18" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="3"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="3"/>
+      <c r="P18" s="3"/>
+      <c r="Q18" s="3"/>
+      <c r="R18" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C19" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="E19" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+      <c r="M19" s="3"/>
+      <c r="N19" s="3"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="3"/>
+      <c r="Q19" s="3"/>
+      <c r="R19" s="5" t="s">
+        <v>109</v>
+      </c>
+    </row>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="28">
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:E1"/>
     <mergeCell ref="F1:I1"/>
@@ -1949,6 +2106,14 @@
     <mergeCell ref="F10:Q10"/>
     <mergeCell ref="F11:Q11"/>
     <mergeCell ref="F12:Q12"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="B16:E16"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="J16:Q16"/>
+    <mergeCell ref="R16:R17"/>
+    <mergeCell ref="F18:I18"/>
+    <mergeCell ref="J18:Q18"/>
+    <mergeCell ref="F19:Q19"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Refactored the CPU and added a Top above the CPU
</commit_message>
<xml_diff>
--- a/Docs/CPU_Opcodes.xlsx
+++ b/Docs/CPU_Opcodes.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Opcodes" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="example" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="IO_Map" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="99">
   <si>
     <t xml:space="preserve">INSTRUCTION</t>
   </si>
@@ -276,6 +277,48 @@
   </si>
   <si>
     <t xml:space="preserve">SELF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I/O SPACE MAP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R/W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bits</t>
+  </si>
+  <si>
+    <t xml:space="preserve">W</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LED0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D0=LED1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KEY1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D0=KEY1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7SEG_BOTTOM 2 DIGS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D0-D7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">7SEG_UPPER 1 DIG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D0-D3</t>
   </si>
 </sst>
 </file>
@@ -358,7 +401,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -391,6 +434,10 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -414,7 +461,7 @@
       <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="4.83"/>
@@ -1089,7 +1136,7 @@
   </sheetPr>
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="220" zoomScaleNormal="220" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
@@ -1331,4 +1378,115 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.83"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="D2" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>91</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>95</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>69</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>97</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:D1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
VGA and UART tested and working.
</commit_message>
<xml_diff>
--- a/Docs/CPU_Opcodes.xlsx
+++ b/Docs/CPU_Opcodes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="106">
   <si>
     <t xml:space="preserve">INSTRUCTION</t>
   </si>
@@ -303,6 +303,9 @@
     <t xml:space="preserve">D0=LED1</t>
   </si>
   <si>
+    <t xml:space="preserve">R</t>
+  </si>
+  <si>
     <t xml:space="preserve">KEY1</t>
   </si>
   <si>
@@ -319,6 +322,24 @@
   </si>
   <si>
     <t xml:space="preserve">D0-D3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART STATUS/CONTROL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UART DATA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0X06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VGA CONTROL/STATUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0X07</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VGA DATA</t>
   </si>
 </sst>
 </file>
@@ -352,12 +373,18 @@
       <family val="0"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -401,7 +428,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -434,8 +461,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -461,7 +500,7 @@
       <selection pane="topLeft" activeCell="D23" activeCellId="0" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="12.07"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="2" style="0" width="4.83"/>
@@ -1385,33 +1424,33 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="7.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="5.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-    </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="8" t="s">
         <v>87</v>
       </c>
       <c r="C2" s="0" t="s">
@@ -1421,11 +1460,11 @@
         <v>89</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="8" t="s">
         <v>90</v>
       </c>
       <c r="C3" s="0" t="s">
@@ -1435,46 +1474,102 @@
         <v>92</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B5" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" s="0" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>90</v>
-      </c>
       <c r="C5" s="0" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>90</v>
+      <c r="B6" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="C6" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C7" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="D6" s="0" t="s">
-        <v>98</v>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Timer Unit added and tested working
</commit_message>
<xml_diff>
--- a/Docs/CPU_Opcodes.xlsx
+++ b/Docs/CPU_Opcodes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="116">
   <si>
     <t xml:space="preserve">INSTRUCTION</t>
   </si>
@@ -340,6 +340,36 @@
   </si>
   <si>
     <t xml:space="preserve">VGA DATA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0X08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">us COUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0X09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ms COUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0X0A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sec COUNT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0X0B</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NOT USED</t>
+  </si>
+  <si>
+    <t xml:space="preserve">STATUS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D0=RUNNING</t>
   </si>
 </sst>
 </file>
@@ -1424,10 +1454,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
+      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1435,7 +1465,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="8" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="8" width="5.09"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.83"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="12.83"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1570,6 +1600,76 @@
       </c>
       <c r="D10" s="11" t="s">
         <v>97</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C12" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C13" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="C14" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="D14" s="11" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="D15" s="11" t="s">
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Cylon Warrior, J12, Shifter all working
</commit_message>
<xml_diff>
--- a/Docs/CPU_Opcodes.xlsx
+++ b/Docs/CPU_Opcodes.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="130">
   <si>
     <t xml:space="preserve">INSTRUCTION</t>
   </si>
@@ -406,6 +406,12 @@
   </si>
   <si>
     <t xml:space="preserve">J12(2..9) 8 BIT LATCH</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0X0D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J12(25..32) INPUT PORT</t>
   </si>
 </sst>
 </file>
@@ -1709,10 +1715,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1939,6 +1945,18 @@
       </c>
       <c r="D16" s="15"/>
     </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="D17" s="15"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:D1"/>

</xml_diff>